<commit_message>
[BACKEND][INTEGRATION]Finished integration of four modules of training dashboard along with DB and also added minor loading updates...
</commit_message>
<xml_diff>
--- a/php_files/test.xlsx
+++ b/php_files/test.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C2F788-EE4B-4700-B066-D99343D16E5D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{734AF1D1-EBB7-423E-86CD-7F47B1CC499E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="4">
   <si>
-    <t>Jagannath</t>
+    <t>Jagannath Pidaparthy</t>
+  </si>
+  <si>
+    <t>Bikku</t>
+  </si>
+  <si>
+    <t>subbu</t>
+  </si>
+  <si>
+    <t>kammi</t>
   </si>
 </sst>
 </file>
@@ -340,1522 +349,2161 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C137"/>
+  <dimension ref="A1:C195"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>52501</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1">
-        <v>50</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>52502</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>50</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>52503</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>50</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>52504</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C4">
-        <v>50</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>52505</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
       </c>
       <c r="C5">
-        <v>50</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>52506</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>50</v>
+        <v>95.3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>52507</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C7">
-        <v>50</v>
+        <v>97.6</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>52508</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C8">
-        <v>50</v>
+        <v>99.9</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>52509</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
         <v>0</v>
       </c>
       <c r="C9">
-        <v>50</v>
+        <v>102.2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>52510</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>50</v>
+        <v>104.5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>52511</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C11">
-        <v>50</v>
+        <v>106.8</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>52512</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C12">
-        <v>50</v>
+        <v>109.1</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>52513</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
         <v>0</v>
       </c>
       <c r="C13">
-        <v>50</v>
+        <v>111.4</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>52514</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14">
-        <v>50</v>
+        <v>113.7</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>52515</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C15">
-        <v>50</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>52516</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C16">
-        <v>50</v>
+        <v>118.3</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>52517</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
         <v>0</v>
       </c>
       <c r="C17">
-        <v>50</v>
+        <v>120.6</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>52518</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18">
-        <v>50</v>
+        <v>122.9</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>52519</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C19">
-        <v>50</v>
+        <v>125.2</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>52520</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C20">
-        <v>50</v>
+        <v>127.5</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>52521</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
         <v>0</v>
       </c>
       <c r="C21">
-        <v>50</v>
+        <v>129.80000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>52522</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22">
-        <v>50</v>
+        <v>132.1</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>52523</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C23">
-        <v>50</v>
+        <v>134.4</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>52524</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C24">
-        <v>50</v>
+        <v>136.69999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>52525</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
         <v>0</v>
       </c>
       <c r="C25">
-        <v>50</v>
+        <v>139</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>52526</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26">
-        <v>50</v>
+        <v>141.30000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>52527</v>
+        <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C27">
-        <v>50</v>
+        <v>143.6</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>52528</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C28">
-        <v>50</v>
+        <v>145.9</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>52529</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
         <v>0</v>
       </c>
       <c r="C29">
-        <v>50</v>
+        <v>148.19999999999999</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>52530</v>
+        <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C30">
-        <v>50</v>
+        <v>150.5</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>52531</v>
+        <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C31">
-        <v>50</v>
+        <v>152.80000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>52532</v>
+        <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C32">
-        <v>50</v>
+        <v>155.1</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>52533</v>
+        <v>33</v>
       </c>
       <c r="B33" t="s">
         <v>0</v>
       </c>
       <c r="C33">
-        <v>50</v>
+        <v>157.4</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>52534</v>
+        <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C34">
-        <v>50</v>
+        <v>159.69999999999999</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>52535</v>
+        <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C35">
-        <v>50</v>
+        <v>162</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>52536</v>
+        <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C36">
-        <v>50</v>
+        <v>164.3</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>52537</v>
+        <v>37</v>
       </c>
       <c r="B37" t="s">
         <v>0</v>
       </c>
       <c r="C37">
-        <v>50</v>
+        <v>166.6</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>52538</v>
+        <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C38">
-        <v>50</v>
+        <v>168.9</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>52539</v>
+        <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C39">
-        <v>50</v>
+        <v>171.2</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>52540</v>
+        <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C40">
-        <v>50</v>
+        <v>173.5</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>52541</v>
+        <v>41</v>
       </c>
       <c r="B41" t="s">
         <v>0</v>
       </c>
       <c r="C41">
-        <v>50</v>
+        <v>175.8</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>52542</v>
+        <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C42">
-        <v>50</v>
+        <v>178.1</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>52543</v>
+        <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C43">
-        <v>50</v>
+        <v>180.4</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>52544</v>
+        <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C44">
-        <v>50</v>
+        <v>182.7</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>52545</v>
+        <v>45</v>
       </c>
       <c r="B45" t="s">
         <v>0</v>
       </c>
       <c r="C45">
-        <v>50</v>
+        <v>185</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>52546</v>
+        <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C46">
-        <v>50</v>
+        <v>187.3</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>52547</v>
+        <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C47">
-        <v>50</v>
+        <v>189.6</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>52548</v>
+        <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C48">
-        <v>50</v>
+        <v>191.9</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>52549</v>
+        <v>49</v>
       </c>
       <c r="B49" t="s">
         <v>0</v>
       </c>
       <c r="C49">
-        <v>50</v>
+        <v>194.2</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>52550</v>
+        <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C50">
-        <v>50</v>
+        <v>196.5</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>52551</v>
+        <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C51">
-        <v>50</v>
+        <v>198.8</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>52552</v>
+        <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C52">
-        <v>50</v>
+        <v>201.1</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>52553</v>
+        <v>53</v>
       </c>
       <c r="B53" t="s">
         <v>0</v>
       </c>
       <c r="C53">
-        <v>50</v>
+        <v>203.4</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>52554</v>
+        <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C54">
-        <v>50</v>
+        <v>205.7</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>52555</v>
+        <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C55">
-        <v>50</v>
+        <v>208</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>52556</v>
+        <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C56">
-        <v>50</v>
+        <v>210.3</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>52557</v>
+        <v>57</v>
       </c>
       <c r="B57" t="s">
         <v>0</v>
       </c>
       <c r="C57">
-        <v>50</v>
+        <v>212.6</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>52558</v>
+        <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C58">
-        <v>50</v>
+        <v>214.9</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>52559</v>
+        <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C59">
-        <v>50</v>
+        <v>217.2</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>52560</v>
+        <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C60">
-        <v>50</v>
+        <v>219.5</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>52561</v>
+        <v>61</v>
       </c>
       <c r="B61" t="s">
         <v>0</v>
       </c>
       <c r="C61">
-        <v>50</v>
+        <v>221.8</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>52562</v>
+        <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C62">
-        <v>50</v>
+        <v>224.1</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>52563</v>
+        <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C63">
-        <v>50</v>
+        <v>226.4</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>52564</v>
+        <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C64">
-        <v>50</v>
+        <v>228.7</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>52565</v>
+        <v>65</v>
       </c>
       <c r="B65" t="s">
         <v>0</v>
       </c>
       <c r="C65">
-        <v>50</v>
+        <v>231</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>52566</v>
+        <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C66">
-        <v>50</v>
+        <v>233.3</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>52567</v>
+        <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C67">
-        <v>50</v>
+        <v>235.6</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>52568</v>
+        <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C68">
-        <v>50</v>
+        <v>237.9</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>52569</v>
+        <v>69</v>
       </c>
       <c r="B69" t="s">
         <v>0</v>
       </c>
       <c r="C69">
-        <v>50</v>
+        <v>240.2</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>52570</v>
+        <v>70</v>
       </c>
       <c r="B70" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C70">
-        <v>50</v>
+        <v>242.5</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>52571</v>
+        <v>71</v>
       </c>
       <c r="B71" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C71">
-        <v>50</v>
+        <v>244.8</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>52572</v>
+        <v>72</v>
       </c>
       <c r="B72" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C72">
-        <v>50</v>
+        <v>247.1</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>52573</v>
+        <v>73</v>
       </c>
       <c r="B73" t="s">
         <v>0</v>
       </c>
       <c r="C73">
-        <v>50</v>
+        <v>249.4</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>52574</v>
+        <v>74</v>
       </c>
       <c r="B74" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C74">
-        <v>50</v>
+        <v>251.7</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>52575</v>
+        <v>75</v>
       </c>
       <c r="B75" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C75">
-        <v>50</v>
+        <v>254</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>52576</v>
+        <v>76</v>
       </c>
       <c r="B76" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C76">
-        <v>50</v>
+        <v>256.3</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>52577</v>
+        <v>77</v>
       </c>
       <c r="B77" t="s">
         <v>0</v>
       </c>
       <c r="C77">
-        <v>50</v>
+        <v>258.60000000000002</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>52578</v>
+        <v>78</v>
       </c>
       <c r="B78" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C78">
-        <v>50</v>
+        <v>260.89999999999998</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>52579</v>
+        <v>79</v>
       </c>
       <c r="B79" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C79">
-        <v>50</v>
+        <v>263.2</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>52580</v>
+        <v>80</v>
       </c>
       <c r="B80" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C80">
-        <v>50</v>
+        <v>265.5</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>52581</v>
+        <v>81</v>
       </c>
       <c r="B81" t="s">
         <v>0</v>
       </c>
       <c r="C81">
-        <v>50</v>
+        <v>267.8</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>52582</v>
+        <v>82</v>
       </c>
       <c r="B82" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C82">
-        <v>50</v>
+        <v>270.10000000000002</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>52583</v>
+        <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C83">
-        <v>50</v>
+        <v>272.39999999999998</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>52584</v>
+        <v>84</v>
       </c>
       <c r="B84" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C84">
-        <v>50</v>
+        <v>274.7</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>52585</v>
+        <v>85</v>
       </c>
       <c r="B85" t="s">
         <v>0</v>
       </c>
       <c r="C85">
-        <v>50</v>
+        <v>277</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>52586</v>
+        <v>86</v>
       </c>
       <c r="B86" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C86">
-        <v>50</v>
+        <v>279.3</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>52587</v>
+        <v>87</v>
       </c>
       <c r="B87" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C87">
-        <v>50</v>
+        <v>281.60000000000002</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>52588</v>
+        <v>88</v>
       </c>
       <c r="B88" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C88">
-        <v>50</v>
+        <v>283.89999999999998</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>52589</v>
+        <v>89</v>
       </c>
       <c r="B89" t="s">
         <v>0</v>
       </c>
       <c r="C89">
-        <v>50</v>
+        <v>286.2</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>52590</v>
+        <v>90</v>
       </c>
       <c r="B90" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C90">
-        <v>50</v>
+        <v>288.5</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>52591</v>
+        <v>91</v>
       </c>
       <c r="B91" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C91">
-        <v>50</v>
+        <v>290.8</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>52592</v>
+        <v>92</v>
       </c>
       <c r="B92" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C92">
-        <v>50</v>
+        <v>293.10000000000002</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>52593</v>
+        <v>93</v>
       </c>
       <c r="B93" t="s">
         <v>0</v>
       </c>
       <c r="C93">
-        <v>50</v>
+        <v>295.39999999999998</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>52594</v>
+        <v>94</v>
       </c>
       <c r="B94" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C94">
-        <v>50</v>
+        <v>297.7</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>52595</v>
+        <v>95</v>
       </c>
       <c r="B95" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C95">
-        <v>50</v>
+        <v>300</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>52596</v>
+        <v>96</v>
       </c>
       <c r="B96" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C96">
-        <v>50</v>
+        <v>302.3</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>52597</v>
+        <v>97</v>
       </c>
       <c r="B97" t="s">
         <v>0</v>
       </c>
       <c r="C97">
-        <v>50</v>
+        <v>304.60000000000002</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>52598</v>
+        <v>98</v>
       </c>
       <c r="B98" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C98">
-        <v>50</v>
+        <v>306.89999999999998</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>52599</v>
+        <v>99</v>
       </c>
       <c r="B99" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C99">
-        <v>50</v>
+        <v>309.2</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>52600</v>
+        <v>100</v>
       </c>
       <c r="B100" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C100">
-        <v>50</v>
+        <v>311.5</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>52601</v>
+        <v>101</v>
       </c>
       <c r="B101" t="s">
         <v>0</v>
       </c>
       <c r="C101">
-        <v>50</v>
+        <v>313.8</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>52602</v>
+        <v>102</v>
       </c>
       <c r="B102" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C102">
-        <v>50</v>
+        <v>316.10000000000002</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>52603</v>
+        <v>103</v>
       </c>
       <c r="B103" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C103">
-        <v>50</v>
+        <v>318.39999999999998</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>52604</v>
+        <v>104</v>
       </c>
       <c r="B104" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C104">
-        <v>50</v>
+        <v>320.7</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>52605</v>
+        <v>105</v>
       </c>
       <c r="B105" t="s">
         <v>0</v>
       </c>
       <c r="C105">
-        <v>50</v>
+        <v>323</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>52606</v>
+        <v>106</v>
       </c>
       <c r="B106" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C106">
-        <v>50</v>
+        <v>325.3</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>52607</v>
+        <v>107</v>
       </c>
       <c r="B107" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C107">
-        <v>50</v>
+        <v>327.60000000000002</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>52608</v>
+        <v>108</v>
       </c>
       <c r="B108" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C108">
-        <v>50</v>
+        <v>329.9</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>52609</v>
+        <v>109</v>
       </c>
       <c r="B109" t="s">
         <v>0</v>
       </c>
       <c r="C109">
-        <v>50</v>
+        <v>332.2</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>52610</v>
+        <v>110</v>
       </c>
       <c r="B110" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C110">
-        <v>50</v>
+        <v>334.5</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>52611</v>
+        <v>111</v>
       </c>
       <c r="B111" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C111">
-        <v>50</v>
+        <v>336.8</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>52612</v>
+        <v>112</v>
       </c>
       <c r="B112" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C112">
-        <v>50</v>
+        <v>339.1</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>52613</v>
+        <v>113</v>
       </c>
       <c r="B113" t="s">
         <v>0</v>
       </c>
       <c r="C113">
-        <v>50</v>
+        <v>341.4</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>52614</v>
+        <v>114</v>
       </c>
       <c r="B114" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C114">
-        <v>50</v>
+        <v>343.7</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>52615</v>
+        <v>115</v>
       </c>
       <c r="B115" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C115">
-        <v>50</v>
+        <v>346</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>52616</v>
+        <v>116</v>
       </c>
       <c r="B116" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C116">
-        <v>50</v>
+        <v>348.3</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117">
-        <v>52617</v>
+        <v>117</v>
       </c>
       <c r="B117" t="s">
         <v>0</v>
       </c>
       <c r="C117">
-        <v>50</v>
+        <v>350.6</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118">
-        <v>52618</v>
+        <v>118</v>
       </c>
       <c r="B118" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C118">
-        <v>50</v>
+        <v>352.9</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119">
-        <v>52619</v>
+        <v>119</v>
       </c>
       <c r="B119" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C119">
-        <v>50</v>
+        <v>355.2</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>52620</v>
+        <v>120</v>
       </c>
       <c r="B120" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C120">
-        <v>50</v>
+        <v>357.5</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121">
-        <v>52621</v>
+        <v>121</v>
       </c>
       <c r="B121" t="s">
         <v>0</v>
       </c>
       <c r="C121">
-        <v>50</v>
+        <v>359.8</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122">
-        <v>52622</v>
+        <v>122</v>
       </c>
       <c r="B122" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C122">
-        <v>50</v>
+        <v>362.1</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123">
-        <v>52623</v>
+        <v>123</v>
       </c>
       <c r="B123" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C123">
-        <v>50</v>
+        <v>364.4</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124">
-        <v>52624</v>
+        <v>124</v>
       </c>
       <c r="B124" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C124">
-        <v>50</v>
+        <v>366.7</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125">
-        <v>52625</v>
+        <v>125</v>
       </c>
       <c r="B125" t="s">
         <v>0</v>
       </c>
       <c r="C125">
-        <v>50</v>
+        <v>369</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126">
-        <v>52626</v>
+        <v>126</v>
       </c>
       <c r="B126" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C126">
-        <v>50</v>
+        <v>371.3</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127">
-        <v>52627</v>
+        <v>127</v>
       </c>
       <c r="B127" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C127">
-        <v>50</v>
+        <v>373.6</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128">
-        <v>52628</v>
+        <v>128</v>
       </c>
       <c r="B128" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C128">
-        <v>50</v>
+        <v>375.9</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129">
-        <v>52629</v>
+        <v>129</v>
       </c>
       <c r="B129" t="s">
         <v>0</v>
       </c>
       <c r="C129">
-        <v>50</v>
+        <v>378.2</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130">
-        <v>52630</v>
+        <v>130</v>
       </c>
       <c r="B130" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C130">
-        <v>50</v>
+        <v>380.5</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131">
-        <v>52631</v>
+        <v>131</v>
       </c>
       <c r="B131" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C131">
-        <v>50</v>
+        <v>382.8</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132">
-        <v>52632</v>
+        <v>132</v>
       </c>
       <c r="B132" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C132">
-        <v>50</v>
+        <v>385.1</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133">
-        <v>52633</v>
+        <v>133</v>
       </c>
       <c r="B133" t="s">
         <v>0</v>
       </c>
       <c r="C133">
-        <v>50</v>
+        <v>387.4</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134">
-        <v>52634</v>
+        <v>134</v>
       </c>
       <c r="B134" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C134">
-        <v>50</v>
+        <v>389.7</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135">
-        <v>52635</v>
+        <v>135</v>
       </c>
       <c r="B135" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C135">
-        <v>50</v>
+        <v>392</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136">
-        <v>52636</v>
+        <v>136</v>
       </c>
       <c r="B136" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C136">
-        <v>50</v>
+        <v>394.3</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137">
-        <v>52637</v>
+        <v>137</v>
       </c>
       <c r="B137" t="s">
         <v>0</v>
       </c>
       <c r="C137">
-        <v>50</v>
+        <v>396.6</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>138</v>
+      </c>
+      <c r="B138" t="s">
+        <v>1</v>
+      </c>
+      <c r="C138">
+        <v>398.9</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>139</v>
+      </c>
+      <c r="B139" t="s">
+        <v>2</v>
+      </c>
+      <c r="C139">
+        <v>401.2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>140</v>
+      </c>
+      <c r="B140" t="s">
+        <v>3</v>
+      </c>
+      <c r="C140">
+        <v>403.5</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>141</v>
+      </c>
+      <c r="B141" t="s">
+        <v>0</v>
+      </c>
+      <c r="C141">
+        <v>405.8</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>142</v>
+      </c>
+      <c r="B142" t="s">
+        <v>1</v>
+      </c>
+      <c r="C142">
+        <v>408.1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>143</v>
+      </c>
+      <c r="B143" t="s">
+        <v>2</v>
+      </c>
+      <c r="C143">
+        <v>410.4</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>144</v>
+      </c>
+      <c r="B144" t="s">
+        <v>3</v>
+      </c>
+      <c r="C144">
+        <v>412.7</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>145</v>
+      </c>
+      <c r="B145" t="s">
+        <v>0</v>
+      </c>
+      <c r="C145">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>146</v>
+      </c>
+      <c r="B146" t="s">
+        <v>1</v>
+      </c>
+      <c r="C146">
+        <v>417.3</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>147</v>
+      </c>
+      <c r="B147" t="s">
+        <v>2</v>
+      </c>
+      <c r="C147">
+        <v>419.6</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>148</v>
+      </c>
+      <c r="B148" t="s">
+        <v>3</v>
+      </c>
+      <c r="C148">
+        <v>421.9</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>149</v>
+      </c>
+      <c r="B149" t="s">
+        <v>0</v>
+      </c>
+      <c r="C149">
+        <v>424.2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>150</v>
+      </c>
+      <c r="B150" t="s">
+        <v>1</v>
+      </c>
+      <c r="C150">
+        <v>426.5</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>151</v>
+      </c>
+      <c r="B151" t="s">
+        <v>2</v>
+      </c>
+      <c r="C151">
+        <v>428.8</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>152</v>
+      </c>
+      <c r="B152" t="s">
+        <v>3</v>
+      </c>
+      <c r="C152">
+        <v>431.1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>153</v>
+      </c>
+      <c r="B153" t="s">
+        <v>0</v>
+      </c>
+      <c r="C153">
+        <v>433.4</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>154</v>
+      </c>
+      <c r="B154" t="s">
+        <v>1</v>
+      </c>
+      <c r="C154">
+        <v>435.7</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>155</v>
+      </c>
+      <c r="B155" t="s">
+        <v>2</v>
+      </c>
+      <c r="C155">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>156</v>
+      </c>
+      <c r="B156" t="s">
+        <v>3</v>
+      </c>
+      <c r="C156">
+        <v>440.3</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>157</v>
+      </c>
+      <c r="B157" t="s">
+        <v>0</v>
+      </c>
+      <c r="C157">
+        <v>442.6</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>158</v>
+      </c>
+      <c r="B158" t="s">
+        <v>1</v>
+      </c>
+      <c r="C158">
+        <v>444.9</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>159</v>
+      </c>
+      <c r="B159" t="s">
+        <v>2</v>
+      </c>
+      <c r="C159">
+        <v>447.2</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>160</v>
+      </c>
+      <c r="B160" t="s">
+        <v>3</v>
+      </c>
+      <c r="C160">
+        <v>449.5</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>161</v>
+      </c>
+      <c r="B161" t="s">
+        <v>0</v>
+      </c>
+      <c r="C161">
+        <v>451.8</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>162</v>
+      </c>
+      <c r="B162" t="s">
+        <v>1</v>
+      </c>
+      <c r="C162">
+        <v>454.1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>163</v>
+      </c>
+      <c r="B163" t="s">
+        <v>2</v>
+      </c>
+      <c r="C163">
+        <v>456.4</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>164</v>
+      </c>
+      <c r="B164" t="s">
+        <v>3</v>
+      </c>
+      <c r="C164">
+        <v>458.7</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>165</v>
+      </c>
+      <c r="B165" t="s">
+        <v>0</v>
+      </c>
+      <c r="C165">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>166</v>
+      </c>
+      <c r="B166" t="s">
+        <v>1</v>
+      </c>
+      <c r="C166">
+        <v>463.3</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>167</v>
+      </c>
+      <c r="B167" t="s">
+        <v>2</v>
+      </c>
+      <c r="C167">
+        <v>465.6</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>168</v>
+      </c>
+      <c r="B168" t="s">
+        <v>3</v>
+      </c>
+      <c r="C168">
+        <v>467.9</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>169</v>
+      </c>
+      <c r="B169" t="s">
+        <v>0</v>
+      </c>
+      <c r="C169">
+        <v>470.2</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>170</v>
+      </c>
+      <c r="B170" t="s">
+        <v>1</v>
+      </c>
+      <c r="C170">
+        <v>472.5</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>171</v>
+      </c>
+      <c r="B171" t="s">
+        <v>2</v>
+      </c>
+      <c r="C171">
+        <v>474.8</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>172</v>
+      </c>
+      <c r="B172" t="s">
+        <v>3</v>
+      </c>
+      <c r="C172">
+        <v>477.1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>173</v>
+      </c>
+      <c r="B173" t="s">
+        <v>0</v>
+      </c>
+      <c r="C173">
+        <v>479.4</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>174</v>
+      </c>
+      <c r="B174" t="s">
+        <v>1</v>
+      </c>
+      <c r="C174">
+        <v>481.7</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>175</v>
+      </c>
+      <c r="B175" t="s">
+        <v>2</v>
+      </c>
+      <c r="C175">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>176</v>
+      </c>
+      <c r="B176" t="s">
+        <v>3</v>
+      </c>
+      <c r="C176">
+        <v>486.3</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>177</v>
+      </c>
+      <c r="B177" t="s">
+        <v>0</v>
+      </c>
+      <c r="C177">
+        <v>488.6</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>178</v>
+      </c>
+      <c r="B178" t="s">
+        <v>1</v>
+      </c>
+      <c r="C178">
+        <v>490.9</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>179</v>
+      </c>
+      <c r="B179" t="s">
+        <v>2</v>
+      </c>
+      <c r="C179">
+        <v>493.2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>180</v>
+      </c>
+      <c r="B180" t="s">
+        <v>3</v>
+      </c>
+      <c r="C180">
+        <v>495.5</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>181</v>
+      </c>
+      <c r="B181" t="s">
+        <v>0</v>
+      </c>
+      <c r="C181">
+        <v>497.8</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>182</v>
+      </c>
+      <c r="B182" t="s">
+        <v>1</v>
+      </c>
+      <c r="C182">
+        <v>500.1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>183</v>
+      </c>
+      <c r="B183" t="s">
+        <v>2</v>
+      </c>
+      <c r="C183">
+        <v>502.4</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>184</v>
+      </c>
+      <c r="B184" t="s">
+        <v>3</v>
+      </c>
+      <c r="C184">
+        <v>504.7</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>185</v>
+      </c>
+      <c r="B185" t="s">
+        <v>0</v>
+      </c>
+      <c r="C185">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>186</v>
+      </c>
+      <c r="B186" t="s">
+        <v>1</v>
+      </c>
+      <c r="C186">
+        <v>509.3</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>187</v>
+      </c>
+      <c r="B187" t="s">
+        <v>2</v>
+      </c>
+      <c r="C187">
+        <v>511.6</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>188</v>
+      </c>
+      <c r="B188" t="s">
+        <v>3</v>
+      </c>
+      <c r="C188">
+        <v>513.9</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>189</v>
+      </c>
+      <c r="B189" t="s">
+        <v>0</v>
+      </c>
+      <c r="C189">
+        <v>516.20000000000005</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>190</v>
+      </c>
+      <c r="B190" t="s">
+        <v>1</v>
+      </c>
+      <c r="C190">
+        <v>518.5</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>191</v>
+      </c>
+      <c r="B191" t="s">
+        <v>2</v>
+      </c>
+      <c r="C191">
+        <v>520.79999999999995</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>192</v>
+      </c>
+      <c r="B192" t="s">
+        <v>3</v>
+      </c>
+      <c r="C192">
+        <v>523.1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>193</v>
+      </c>
+      <c r="B193" t="s">
+        <v>0</v>
+      </c>
+      <c r="C193">
+        <v>525.4</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>194</v>
+      </c>
+      <c r="B194" t="s">
+        <v>1</v>
+      </c>
+      <c r="C194">
+        <v>527.70000000000005</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>195</v>
+      </c>
+      <c r="B195" t="s">
+        <v>2</v>
+      </c>
+      <c r="C195">
+        <v>530</v>
       </c>
     </row>
   </sheetData>

</xml_diff>